<commit_message>
add climate categorisation source tables
</commit_message>
<xml_diff>
--- a/data-input/regulation-tables/reg-table_1_climate-categories_nonagri.xlsx
+++ b/data-input/regulation-tables/reg-table_1_climate-categories_nonagri.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petr/cwork/esiftagging/data-input/regulation-tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A24D271-ECBD-194E-AE23-CA2B6A2AE1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1080CBEB-BEEC-C14A-A883-7FCEBB692E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35400" yWindow="-6760" windowWidth="32540" windowHeight="20980" xr2:uid="{1A82F363-8550-0B4B-985E-30F02D0D30EE}"/>
+    <workbookView xWindow="35400" yWindow="-6760" windowWidth="32540" windowHeight="20980" activeTab="1" xr2:uid="{1A82F363-8550-0B4B-985E-30F02D0D30EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="About" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="149">
   <si>
     <t>1.</t>
   </si>
@@ -479,6 +480,9 @@
   </si>
   <si>
     <t>Information and communication</t>
+  </si>
+  <si>
+    <t>source: https://eur-lex.europa.eu/legal-content/EN/TXT/HTML/?uri=CELEX:32014R0215&amp;from=EN#d1e32-71-1</t>
   </si>
 </sst>
 </file>
@@ -844,7 +848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C149850-7262-EE41-B3BD-403294C6C704}">
   <dimension ref="A1:C143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A51" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2358,4 +2362,24 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60EB569A-9E44-B246-8543-9CA921B996E5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>